<commit_message>
Tela de cadastro finalizada no backlog
</commit_message>
<xml_diff>
--- a/documentação/Backlog_Shitech.xlsx
+++ b/documentação/Backlog_Shitech.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28122"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/66ff8a83318b4257/SPTECH/1Semestre/Sprint2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bandteccom-my.sharepoint.com/personal/felipe_osouza_sptech_school/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{67F666C3-C1D6-4339-AC43-A4908378D7F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EECF8E91-CBCB-44A6-B852-C6475009A8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,12 +36,36 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="41">
+  <si>
+    <t>Requisito</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>Classificação</t>
+  </si>
+  <si>
+    <t>Funcional</t>
+  </si>
+  <si>
+    <t>TELA INICIAL(1.0)</t>
+  </si>
+  <si>
+    <t>1.1. TELA INICIAL. ( Informações da tela)</t>
+  </si>
+  <si>
+    <t>Essencial</t>
+  </si>
+  <si>
+    <t>Sim</t>
+  </si>
   <si>
     <t>No parte superior da tela inicial haverá uma barra de navegação (1.2). Abaixo terá 3 botões que irão redirecionar o usuário para partes específicas do site, sendo eles da esquerda para direita: QUEM SOMOS, NOSSO PROPÓSITO E SIMULADOR(1.3).  Seção de PRODUTO DISPONÍVEL(1.4). Seção de QUEM SOMOS E NOSSO PROPÓSITO(1.5).  O simulador financeiro (1.6) e ao final o footer do site(1.7)</t>
   </si>
   <si>
-    <t>TELA INICIAL(1.0)</t>
+    <t>1.2. TELA INICIAL. (Barra de navegação)</t>
   </si>
   <si>
     <t>A barra de navegação será composta pelos seguintes itens da esquerda para direita: Um input para o usuário executar pesquisas dentro do site, na parte central a logo do projeto e ao final, um texto de "bem-vindo" com outro texto "entrar" logo abaixo, a direita desses dois textos terá um icone de login.</t>
@@ -50,34 +74,19 @@
     <t>IMAGEM DE ILUSTRAÇÃO ABAIXO</t>
   </si>
   <si>
-    <t>1.1. TELA INICIAL. ( Informações da tela)</t>
-  </si>
-  <si>
-    <t>1.2. TELA INICIAL. (Barra de navegação)</t>
-  </si>
-  <si>
     <t>1.3. TELA INICIAL. (BOTÕES SUPERIORES)</t>
   </si>
   <si>
-    <t>Essencial</t>
+    <t>Haverá 3 botões da esquerda para direita, sendo eles: QUEM SOMOS, que irá direcionar o usuário para a parte de "quem somos"(1.5).O segundo botão será NOSSO PROPÓSITO que irá direcionar o usuário para a parte "nosso propósito"(1.5), Por fim terá um botão SIMULAR que irá direcionar o usuário para a parte de simulação (1.6)</t>
+  </si>
+  <si>
+    <t>1.4. TELA INICIAL. (PRODUTO DISPONÍVEL)</t>
   </si>
   <si>
     <t>Importante</t>
   </si>
   <si>
-    <t>Haverá 3 botões da esquerda para direita, sendo eles: QUEM SOMOS, que irá direcionar o usuário para a parte de "quem somos"(1.5).O segundo botão será NOSSO PROPÓSITO que irá direcionar o usuário para a parte "nosso propósito"(1.5), Por fim terá um botão SIMULAR que irá direcionar o usuário para a parte de simulação (1.6)</t>
-  </si>
-  <si>
-    <t>Classificação</t>
-  </si>
-  <si>
-    <t>Funcional</t>
-  </si>
-  <si>
-    <t>Sim</t>
-  </si>
-  <si>
-    <t>1.4. TELA INICIAL. (PRODUTO DISPONÍVEL)</t>
+    <t>Não</t>
   </si>
   <si>
     <t>Possui um título "PRODUTO DISPONÍVEL". Abaixo haverá uma divisão de dois blocos na parte central dessa seção. A esquerda terá um subtitulo "Aumente a eficiência do seu cultivo em até 40% !!!" e 2 textos logo abaixo, sendo eles respectivamente: "Com nossos sensores que auxiliam na adequação de ambiente em cultivo de Fungos" e "Fique à frente do mercado com nosso inovador sistema de sensores, garantindo a segurança e a integridade do seu cultivo, promovendo o ambiente perfeito para a criação de seus fungos!". O segundo bloco a direita terá a imagem de uma plantação de cogumelo</t>
@@ -175,20 +184,64 @@
     </r>
   </si>
   <si>
-    <t>Descrição</t>
-  </si>
-  <si>
-    <t>Requisito</t>
-  </si>
-  <si>
-    <t>Não</t>
+    <t>TELA LOGIN (2.0)</t>
+  </si>
+  <si>
+    <t>2.1.TELA LOGIN</t>
+  </si>
+  <si>
+    <t>A tela de login será composta na parte superior pelo nome SHITECH, em baixo um texto escrito login seguido da logo da SHITECH, abaixo da logo ficará os campos de entrada de email e senha, e na parte inferior ficará o botão de Entrar, a baixo ficará a opção de esquecer a senha e a opção de se cadastrar.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IMAGEM DE ILUSTRAÇÃO ABAIXO 
+(Cor de fundo: #A68A64 Cor das letras: #936639) </t>
+  </si>
+  <si>
+    <t>2.2. LOGO DA TELA DE CADASTRO</t>
+  </si>
+  <si>
+    <t>2.3. INPUTS DE EMAIL E SENHA</t>
+  </si>
+  <si>
+    <t>2.4. BOTÃO DE ENTRADA 
+(Cor do Botão: #936639 Border Radius: 100px)</t>
+  </si>
+  <si>
+    <t>2.5. BOTÕES DE ESQUECI A SENHA E CADASTRO</t>
+  </si>
+  <si>
+    <t>3.0 TELA DE CADASTRO</t>
+  </si>
+  <si>
+    <t>3.0. TELA DE CADASTRO (INFORMAÇÕES DA TELA)</t>
+  </si>
+  <si>
+    <t>Essa tela será a tela onde o usuário irá se cadastrar no site. Na parte central da tela terá um quadrado branco. Na parte superior do quadrado, alinhado na parte central do eixo horizontal, terá a logo da SHITECH (3.1). Logo abaixo, na parte central estarão os inputs para cadastro (3.2). Na parte final, terá um botão de "CADASTRAR" e abaixo deste botão outro de "Já possui uma conta?" (3.3).</t>
+  </si>
+  <si>
+    <t>3.1. TELA DE CADASTRO (LOGO)</t>
+  </si>
+  <si>
+    <t>3.3. TELA DE CADASTRO (INPUTS)</t>
+  </si>
+  <si>
+    <t>Os inputs são dividos em 3 linhas. Na primeira linha teremos 2 inputs: Razão Social e CNPJ. Na segunda linha teremos 2 inputs: Email e telefone. A ultima linha será composta por 2 inputs: Senha e Confirme a senha.</t>
+  </si>
+  <si>
+    <t>Temos que definir a quantidade de caracteres dos inputs</t>
+  </si>
+  <si>
+    <t>3.4. TELA DE CADASTRO (BOTÕES).</t>
+  </si>
+  <si>
+    <t>Teremos 2 botões abaixo dos inputs. O botão "CADASTRAR" irá direcionar o usuário para a tela de login(2.0) caso o mesmo já tenha preenchido todos os dados corretamente. O botão "Já possui uma conta?" irá direcionar o usuário para a tela do login (2.0)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +290,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -269,21 +337,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="11">
+  <borders count="20">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -341,20 +412,90 @@
     <border>
       <left/>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
       </left>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -362,27 +503,65 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color indexed="64"/>
+      <right style="medium">
+        <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -393,73 +572,153 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="distributed"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -471,6 +730,253 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8B368"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8B368"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8B368"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8B368"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF8B368"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.749961851863155"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
         </patternFill>
       </fill>
     </dxf>
@@ -494,6 +1000,20 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
         <color auto="1"/>
       </font>
@@ -524,6 +1044,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFD1CECB"/>
       <color rgb="FFFFFF99"/>
       <color rgb="FFF8B368"/>
       <color rgb="FFFC8C04"/>
@@ -546,19 +1067,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1621762</xdr:colOff>
+      <xdr:colOff>1526512</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3079087</xdr:colOff>
+      <xdr:colOff>2983837</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>247650</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="30" name="CaixaDeTexto 29">
+        <xdr:cNvPr id="15" name="CaixaDeTexto 29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3203C1BE-9807-8E08-1091-223BB85D5323}"/>
@@ -572,7 +1093,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3526762" y="0"/>
+          <a:off x="3402937" y="0"/>
           <a:ext cx="1457325" cy="247650"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -607,15 +1128,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10389</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>163657</xdr:rowOff>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3879272</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>296388</xdr:rowOff>
+      <xdr:colOff>3743325</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -625,7 +1146,7 @@
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{30FD0D6D-B278-2070-C949-F087481EF506}"/>
             </a:ext>
             <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
-              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{8B9DEF87-FD18-2FAA-C377-3E28D335EB0B}"/>
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{3203C1BE-9807-8E08-1091-223BB85D5323}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -641,8 +1162,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1915389" y="4579793"/>
-          <a:ext cx="3868883" cy="314572"/>
+          <a:off x="1876425" y="4600575"/>
+          <a:ext cx="3743325" cy="314325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -654,13 +1175,13 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>10390</xdr:colOff>
+      <xdr:colOff>865</xdr:colOff>
       <xdr:row>11</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3762376</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>8659</xdr:rowOff>
     </xdr:to>
@@ -688,8 +1209,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1915390" y="6416386"/>
-          <a:ext cx="3868884" cy="277091"/>
+          <a:off x="1877290" y="6410325"/>
+          <a:ext cx="3761511" cy="275359"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -701,19 +1222,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1731</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>17318</xdr:colOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
       <xdr:row>16</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Imagem 6">
+        <xdr:cNvPr id="16" name="Imagem 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A13D49F8-E2EB-58A8-3B97-8A644B4AE9FB}"/>
@@ -735,8 +1256,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1906731" y="8918864"/>
-          <a:ext cx="3894860" cy="2121478"/>
+          <a:off x="1876425" y="8953500"/>
+          <a:ext cx="3762375" cy="2124075"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -748,19 +1269,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>9524</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>1220240</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Imagem 10">
+        <xdr:cNvPr id="10" name="Imagem 10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C66D8191-F090-AE1C-E570-C84297019FB7}"/>
@@ -782,8 +1303,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1914524" y="14374091"/>
-          <a:ext cx="3869749" cy="1220240"/>
+          <a:off x="1876425" y="14592300"/>
+          <a:ext cx="3762375" cy="1219200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -795,15 +1316,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>8660</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>181840</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>24</xdr:row>
-      <xdr:rowOff>17317</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -829,8 +1350,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1913660" y="19985181"/>
-          <a:ext cx="3870614" cy="2060863"/>
+          <a:off x="1876425" y="20402550"/>
+          <a:ext cx="3771900" cy="2076450"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -849,8 +1370,8 @@
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>8659</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>5546</xdr:rowOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>1081871</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -889,22 +1410,25 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1766240</xdr:colOff>
+      <xdr:colOff>1632890</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>121476</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>3004704</xdr:colOff>
+      <xdr:colOff>2871354</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>69735</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="61" name="Imagem 60">
+        <xdr:cNvPr id="13" name="Imagem 60">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00BA48B1-FFF9-4CF3-1C8E-0F892640B173}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{31A50755-1134-7689-BE33-375DEED707B4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -920,8 +1444,431 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3671240" y="121476"/>
-          <a:ext cx="1238464" cy="1238464"/>
+          <a:off x="3509315" y="121476"/>
+          <a:ext cx="1238464" cy="1234134"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3762375</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>2447925</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="19" name="Imagem 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DAB7A1D-70B7-6033-8643-C3DB1A965B53}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{00BA48B1-FFF9-4CF3-1C8E-0F892640B173}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="34232850"/>
+          <a:ext cx="3771900" cy="2447925"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>3676650</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Imagem 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CDE2F9F-BFE6-83A6-6A4F-55A17FDA071C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{2DAB7A1D-70B7-6033-8643-C3DB1A965B53}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="37080825"/>
+          <a:ext cx="3781425" cy="3676650"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1257300</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="28" name="Imagem 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{780ECF20-52E2-2386-F7CC-6602D0DB39D4}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{7CDE2F9F-BFE6-83A6-6A4F-55A17FDA071C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1866900" y="46101000"/>
+          <a:ext cx="3781425" cy="1362075"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1247775</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>466725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="104" name="Imagem 42">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75BA37D1-4DC4-63C6-C6FE-7B3460C795A5}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5533B5DC-FBED-45A5-B8BC-F6C802C5855C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId11"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1857375" y="29308425"/>
+          <a:ext cx="3810000" cy="2428875"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>4657725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="107" name="Imagem 106">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC2981B7-B36E-B7AB-4647-19CB63161139}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{E03F04B4-E1E5-8708-51C1-2804D90FDA6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="31946850"/>
+          <a:ext cx="3781425" cy="4657725"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3209925</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>1447800</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="108" name="Imagem 107">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5801189A-8878-6C45-EAF9-A9ADE5590529}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{BC2981B7-B36E-B7AB-4647-19CB63161139}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId13"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2295525" y="37014150"/>
+          <a:ext cx="2790825" cy="1276350"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="110" name="Imagem 109">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CA4F7ECD-1243-883A-A0AF-2451D0EF1262}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{5801189A-8878-6C45-EAF9-A9ADE5590529}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId14"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="38681025"/>
+          <a:ext cx="3781425" cy="1590675"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>866775</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="111" name="Imagem 110">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6C0D167-DC09-36DE-3891-3785F7B021BC}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{CA4F7ECD-1243-883A-A0AF-2451D0EF1262}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="40443150"/>
+          <a:ext cx="3771900" cy="876300"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>3752850</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>1495425</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="113" name="Imagem 112">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{92748DB8-6479-48C8-A2F3-335F2A121E8C}"/>
+            </a:ext>
+            <a:ext uri="{147F2762-F138-4A5C-976F-8EAC2B608ADB}">
+              <a16:predDERef xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" pred="{D6C0D167-DC09-36DE-3891-3785F7B021BC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1876425" y="56807100"/>
+          <a:ext cx="3752850" cy="1495425"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -931,10 +1878,6 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1256,574 +2199,751 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="Z8" sqref="Z8"/>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E53" sqref="C53:E55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="19" customWidth="1"/>
-    <col min="3" max="3" width="56.5546875" customWidth="1"/>
-    <col min="4" max="4" width="16.77734375" customWidth="1"/>
-    <col min="5" max="5" width="11.5546875" customWidth="1"/>
-    <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="56.5703125" customWidth="1"/>
+    <col min="4" max="4" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.28515625" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="101.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="15"/>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="17"/>
-    </row>
-    <row r="2" spans="1:9" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="14" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" ht="101.45" customHeight="1">
+      <c r="B1" s="6"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:9" s="4" customFormat="1" ht="30" customHeight="1">
+      <c r="B2" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="16" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
       <c r="A3" s="1"/>
       <c r="B3" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="19"/>
-    </row>
-    <row r="4" spans="1:9" ht="109.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="23" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="109.15" customHeight="1">
       <c r="A4" s="1"/>
       <c r="B4" s="18"/>
-      <c r="C4" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="20" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="21" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C4" s="27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29"/>
+    </row>
+    <row r="5" spans="1:9">
       <c r="A5" s="1"/>
       <c r="B5" s="18"/>
-      <c r="C5" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="19"/>
-    </row>
-    <row r="6" spans="1:9" ht="78.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C5" s="23" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="78.75" customHeight="1">
       <c r="A6" s="1"/>
       <c r="B6" s="18"/>
-      <c r="C6" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E6" s="22" t="s">
-        <v>12</v>
-      </c>
+      <c r="C6" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" ht="14.45" customHeight="1">
       <c r="A7" s="1"/>
       <c r="B7" s="18"/>
-      <c r="C7" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="6"/>
-      <c r="E7" s="22"/>
-    </row>
-    <row r="8" spans="1:9" ht="24" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C7" s="30" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="28"/>
+      <c r="E7" s="29"/>
+    </row>
+    <row r="8" spans="1:9" ht="24" customHeight="1">
       <c r="A8" s="1"/>
       <c r="B8" s="18"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="22"/>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C8" s="36"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+    </row>
+    <row r="9" spans="1:9">
       <c r="A9" s="1"/>
       <c r="B9" s="18"/>
-      <c r="C9" s="11" t="s">
+      <c r="C9" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="26" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="19"/>
-    </row>
-    <row r="10" spans="1:9" ht="90.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E9" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="90.75" customHeight="1">
       <c r="A10" s="1"/>
       <c r="B10" s="18"/>
-      <c r="C10" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E10" s="22" t="s">
-        <v>12</v>
-      </c>
+      <c r="C10" s="27" t="s">
+        <v>13</v>
+      </c>
+      <c r="D10" s="32"/>
+      <c r="E10" s="33"/>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11" s="1"/>
       <c r="B11" s="18"/>
-      <c r="C11" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D11" s="6"/>
-      <c r="E11" s="22"/>
-    </row>
-    <row r="12" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C11" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="32"/>
+      <c r="E11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" ht="21" customHeight="1">
       <c r="A12" s="1"/>
       <c r="B12" s="18"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="22"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="36"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="33"/>
+    </row>
+    <row r="13" spans="1:9">
       <c r="A13" s="1"/>
       <c r="B13" s="18"/>
-      <c r="C13" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="D13" s="12"/>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:9" ht="147.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C13" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="E13" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="147.75" customHeight="1">
       <c r="A14" s="1"/>
       <c r="B14" s="18"/>
-      <c r="C14" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="C14" s="36" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
+    </row>
+    <row r="15" spans="1:9">
       <c r="A15" s="1"/>
       <c r="B15" s="18"/>
-      <c r="C15" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="6"/>
-      <c r="E15" s="22"/>
-    </row>
-    <row r="16" spans="1:9" ht="167.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C15" s="37" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
+    </row>
+    <row r="16" spans="1:9" ht="167.25" customHeight="1">
       <c r="A16" s="1"/>
       <c r="B16" s="18"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="22"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C16" s="36"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="1"/>
       <c r="B17" s="18" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="12"/>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" ht="232.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="E17" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="246.75" customHeight="1">
       <c r="A18" s="1"/>
       <c r="B18" s="18"/>
-      <c r="C18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E18" s="22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" s="32"/>
+      <c r="E18" s="33"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.75" customHeight="1">
       <c r="A19" s="1"/>
       <c r="B19" s="18"/>
-      <c r="C19" s="23" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" s="6"/>
-      <c r="E19" s="22"/>
-    </row>
-    <row r="20" spans="1:5" ht="96" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="39" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="32"/>
+      <c r="E19" s="33"/>
+    </row>
+    <row r="20" spans="1:5" ht="96" customHeight="1">
       <c r="A20" s="1"/>
       <c r="B20" s="18"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="22"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C20" s="36"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="33"/>
+    </row>
+    <row r="21" spans="1:5">
       <c r="A21" s="1"/>
       <c r="B21" s="18"/>
-      <c r="C21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="19"/>
-    </row>
-    <row r="22" spans="1:5" ht="316.8" x14ac:dyDescent="0.3">
+      <c r="C21" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="D21" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="332.25">
       <c r="A22" s="1"/>
       <c r="B22" s="18"/>
-      <c r="C22" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C22" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="32"/>
+      <c r="E22" s="33"/>
+    </row>
+    <row r="23" spans="1:5">
       <c r="A23" s="1"/>
       <c r="B23" s="18"/>
-      <c r="C23" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D23" s="6"/>
-      <c r="E23" s="22"/>
-    </row>
-    <row r="24" spans="1:5" ht="161.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="32"/>
+      <c r="E23" s="33"/>
+    </row>
+    <row r="24" spans="1:5" ht="161.25" customHeight="1">
       <c r="A24" s="1"/>
       <c r="B24" s="18"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="22"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="C24" s="36"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="33"/>
+    </row>
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
       <c r="B25" s="18"/>
-      <c r="C25" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="12"/>
-      <c r="E25" s="12"/>
-    </row>
-    <row r="26" spans="1:5" ht="296.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="291" customHeight="1">
       <c r="A26" s="1"/>
       <c r="B26" s="18"/>
-      <c r="C26" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E26" s="22" t="s">
+      <c r="C26" s="27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="D26" s="32"/>
+      <c r="E26" s="33"/>
+    </row>
+    <row r="27" spans="1:5">
       <c r="A27" s="1"/>
       <c r="B27" s="18"/>
-      <c r="C27" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="6"/>
-      <c r="E27" s="22"/>
-    </row>
-    <row r="28" spans="1:5" ht="85.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="32"/>
+      <c r="E27" s="33"/>
+    </row>
+    <row r="28" spans="1:5" ht="85.5" customHeight="1">
       <c r="A28" s="1"/>
-      <c r="B28" s="24"/>
-      <c r="C28" s="25"/>
-      <c r="D28" s="26"/>
-      <c r="E28" s="27"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B28" s="18"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33"/>
+    </row>
+    <row r="29" spans="1:5" ht="18.75" customHeight="1">
       <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B29" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" ht="75.75" customHeight="1">
       <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="B30" s="21"/>
+      <c r="C30" s="38" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" s="41"/>
+      <c r="E30" s="33"/>
+    </row>
+    <row r="31" spans="1:5" ht="39.75" customHeight="1">
+      <c r="B31" s="21"/>
+      <c r="C31" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="41"/>
+      <c r="E31" s="33"/>
+    </row>
+    <row r="32" spans="1:5" ht="186" customHeight="1">
       <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="21"/>
+      <c r="C32" s="45"/>
+      <c r="D32" s="42"/>
+      <c r="E32" s="35"/>
+    </row>
+    <row r="33" spans="1:5" ht="15" customHeight="1">
       <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B33" s="21"/>
+      <c r="C33" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="D33" s="17"/>
+      <c r="E33" s="14"/>
+    </row>
+    <row r="34" spans="1:5" ht="368.25" customHeight="1">
+      <c r="B34" s="21"/>
+      <c r="D34" s="17"/>
+      <c r="E34" s="14"/>
+    </row>
+    <row r="35" spans="1:5" ht="17.25" customHeight="1">
       <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B35" s="21"/>
+      <c r="C35" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="D35" s="17"/>
+      <c r="E35" s="14"/>
+    </row>
+    <row r="36" spans="1:5" ht="114.75" customHeight="1">
       <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B36" s="21"/>
+      <c r="C36" s="15"/>
+      <c r="D36" s="17"/>
+      <c r="E36" s="14"/>
+    </row>
+    <row r="37" spans="1:5" ht="27" customHeight="1">
       <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B37" s="21"/>
+      <c r="C37" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="D37" s="17"/>
+      <c r="E37" s="14"/>
+    </row>
+    <row r="38" spans="1:5" ht="125.25" customHeight="1">
       <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B38" s="21"/>
+      <c r="D38" s="17"/>
+      <c r="E38" s="14"/>
+    </row>
+    <row r="39" spans="1:5" ht="14.45" customHeight="1">
       <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B39" s="21"/>
+      <c r="C39" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="17"/>
+      <c r="E39" s="14"/>
+    </row>
+    <row r="40" spans="1:5" ht="69" customHeight="1">
       <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B40" s="22"/>
+      <c r="D40" s="17"/>
+      <c r="E40" s="14"/>
+    </row>
+    <row r="41" spans="1:5" ht="15.75" customHeight="1">
       <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B41" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="C41" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" ht="96" customHeight="1">
       <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B42" s="52"/>
+      <c r="C42" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="D42" s="49"/>
+      <c r="E42" s="46"/>
+    </row>
+    <row r="43" spans="1:5" ht="15.75" customHeight="1">
       <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B43" s="52"/>
+      <c r="C43" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="49"/>
+      <c r="E43" s="46"/>
+    </row>
+    <row r="44" spans="1:5" ht="193.5" customHeight="1">
       <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B44" s="52"/>
+      <c r="C44" s="39"/>
+      <c r="D44" s="49"/>
+      <c r="E44" s="46"/>
+    </row>
+    <row r="45" spans="1:5">
       <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B45" s="52"/>
+      <c r="C45" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
       <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B46" s="52"/>
+      <c r="C46" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="49"/>
+      <c r="E46" s="46"/>
+    </row>
+    <row r="47" spans="1:5" ht="290.25" customHeight="1">
       <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B47" s="52"/>
+      <c r="C47" s="36"/>
+      <c r="D47" s="49"/>
+      <c r="E47" s="46"/>
+    </row>
+    <row r="48" spans="1:5">
       <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B48" s="52"/>
+      <c r="C48" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E48" s="25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="57.75">
       <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B49" s="52"/>
+      <c r="C49" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D49" s="49"/>
+      <c r="E49" s="46"/>
+      <c r="G49" s="13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B50" s="52"/>
+      <c r="C50" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D50" s="49"/>
+      <c r="E50" s="46"/>
+    </row>
+    <row r="51" spans="1:7" ht="107.25" customHeight="1">
       <c r="A51" s="1"/>
-      <c r="B51" s="1"/>
-      <c r="C51" s="1"/>
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B51" s="52"/>
+      <c r="C51" s="31"/>
+      <c r="D51" s="51"/>
+      <c r="E51" s="47"/>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" s="1"/>
-      <c r="B52" s="1"/>
-      <c r="C52" s="1"/>
-      <c r="D52" s="1"/>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B52" s="19"/>
+      <c r="C52" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="65.25" customHeight="1">
       <c r="A53" s="1"/>
-      <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
-      <c r="D53" s="1"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B53" s="52"/>
+      <c r="C53" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="D53" s="54"/>
+      <c r="E53" s="55"/>
+    </row>
+    <row r="54" spans="1:7" ht="16.5" customHeight="1">
       <c r="A54" s="1"/>
-      <c r="B54" s="1"/>
-      <c r="C54" s="1"/>
-      <c r="D54" s="1"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="1"/>
-      <c r="B55" s="1"/>
-      <c r="C55" s="1"/>
-      <c r="D55" s="1"/>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="1"/>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="1"/>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57" s="1"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58" s="1"/>
-      <c r="B58" s="1"/>
-      <c r="C58" s="1"/>
-      <c r="D58" s="1"/>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59" s="1"/>
-      <c r="B59" s="1"/>
-      <c r="C59" s="1"/>
-      <c r="D59" s="1"/>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60" s="1"/>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="1"/>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61" s="1"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="1"/>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="1"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="1"/>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63" s="1"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
-      <c r="D63" s="1"/>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="1"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="1"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65" s="1"/>
-      <c r="B65" s="1"/>
-      <c r="C65" s="1"/>
-      <c r="D65" s="1"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66" s="1"/>
-      <c r="B66" s="1"/>
-      <c r="C66" s="1"/>
-      <c r="D66" s="1"/>
+      <c r="B54" s="52"/>
+      <c r="C54" s="40" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="49"/>
+      <c r="E54" s="46"/>
+    </row>
+    <row r="55" spans="1:7" ht="119.25" customHeight="1">
+      <c r="B55" s="57"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="56"/>
+      <c r="E55" s="47"/>
+    </row>
+    <row r="56" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B56" s="11"/>
+    </row>
+    <row r="57" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B57" s="11"/>
+    </row>
+    <row r="58" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B58" s="11"/>
+    </row>
+    <row r="59" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B59" s="11"/>
+    </row>
+    <row r="60" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B60" s="11"/>
+    </row>
+    <row r="61" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B61" s="11"/>
+    </row>
+    <row r="62" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B62" s="11"/>
+    </row>
+    <row r="63" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B63" s="11"/>
+    </row>
+    <row r="64" spans="1:7" ht="14.45" customHeight="1">
+      <c r="B64" s="11"/>
+    </row>
+    <row r="65" spans="2:2" ht="14.45" customHeight="1">
+      <c r="B65" s="11"/>
+    </row>
+    <row r="66" spans="2:2" ht="14.45" customHeight="1">
+      <c r="B66" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="D26:D27"/>
-    <mergeCell ref="E26:E27"/>
-    <mergeCell ref="D18:D20"/>
+  <mergeCells count="19">
+    <mergeCell ref="E30:E32"/>
+    <mergeCell ref="D30:D32"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="D22:D24"/>
     <mergeCell ref="E22:E24"/>
-    <mergeCell ref="B17:B28"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D21:E21"/>
-    <mergeCell ref="D25:E25"/>
-    <mergeCell ref="D6:D8"/>
-    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E26:E28"/>
     <mergeCell ref="D10:D12"/>
     <mergeCell ref="E10:E12"/>
     <mergeCell ref="B3:B16"/>
     <mergeCell ref="E14:E16"/>
     <mergeCell ref="D14:D16"/>
+    <mergeCell ref="D33:D35"/>
+    <mergeCell ref="D36:D38"/>
+    <mergeCell ref="D39:D40"/>
+    <mergeCell ref="B41:B55"/>
+    <mergeCell ref="B17:B28"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="D18:D20"/>
+    <mergeCell ref="B29:B40"/>
   </mergeCells>
-  <conditionalFormatting sqref="D4 D14 D18 D22 D26 D6 D10 D28:D51">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="equal">
+  <conditionalFormatting sqref="D3:D6 D9:D10 D13:D14 D17:D18 D21:D22 D25:D26 D29">
+    <cfRule type="cellIs" dxfId="39" priority="58" operator="equal">
       <formula>"Importante"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="62" operator="equal">
       <formula>"Desejável"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="63" operator="equal">
       <formula>"Essencial"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F4">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="61" operator="equal">
       <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E4 E6 E14 E18 E22 E26 E10 E28:E51">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+  <conditionalFormatting sqref="E3:E6 E9:E10 E13:E14 E17:E18 E21:E22 E29 E37:E38 E25:E26">
+    <cfRule type="cellIs" dxfId="35" priority="59" operator="equal">
       <formula>"Não"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="34" priority="60" operator="equal">
       <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H9">
-    <cfRule type="cellIs" dxfId="2" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="64" operator="equal">
       <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" dxfId="32" priority="47" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="31" priority="48" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="30" priority="49" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="cellIs" dxfId="29" priority="45" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="28" priority="46" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G36">
+    <cfRule type="cellIs" dxfId="27" priority="39" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="26" priority="40" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D30:E30 D33 D36 D39">
+    <cfRule type="cellIs" dxfId="25" priority="33" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="24" priority="34" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" dxfId="23" priority="31" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="22" priority="32" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" dxfId="21" priority="29" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="20" priority="30" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D41">
+    <cfRule type="cellIs" dxfId="19" priority="18" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="18" priority="19" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="17" priority="20" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D45">
+    <cfRule type="cellIs" dxfId="16" priority="15" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="15" priority="16" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="17" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D48">
+    <cfRule type="cellIs" dxfId="13" priority="12" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="14" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D52">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
+      <formula>"Importante"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+      <formula>"Desejável"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
+      <formula>"Essencial"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Sim"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>"Não"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+      <formula>"Sim"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>